<commit_message>
Update Sprint backlog to reflect efforts today
Update the sprint backlog to reflect today's effort
</commit_message>
<xml_diff>
--- a/documentation/Sprint Backlog  Burndown.xlsx
+++ b/documentation/Sprint Backlog  Burndown.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10114"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20405"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/0c751dba731cb2a1/Documents/UWG/2024/Software Engineering 2/Inventory Manager Project/SE2Project/documentation/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jn00041\Documents\GitHub\SE2Project\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="151" documentId="13_ncr:1_{9C9C4265-351C-41A0-89E5-93A08D9C51A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{28BD0E6D-5362-094C-AE02-20C0C1794EB9}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC4E872E-771B-4DF7-AE59-4908DC9F206B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10900" yWindow="1240" windowWidth="29400" windowHeight="17160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="10902" yWindow="1242" windowWidth="29400" windowHeight="17160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,17 +19,6 @@
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -367,13 +356,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>42</c:v>
+                  <c:v>46</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0</c:v>
@@ -1427,18 +1416,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H29"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="146" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16:B20"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.83984375" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
     <col min="1" max="2" width="26" customWidth="1"/>
-    <col min="3" max="3" width="41.6640625" customWidth="1"/>
-    <col min="4" max="4" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="41.68359375" customWidth="1"/>
+    <col min="4" max="4" width="14.47265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
@@ -1456,7 +1445,7 @@
       <c r="G1" s="7"/>
       <c r="H1" s="7"/>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="8"/>
       <c r="B2" s="6"/>
       <c r="C2" s="8"/>
@@ -1474,7 +1463,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="1" t="s">
         <v>10</v>
       </c>
@@ -1485,16 +1474,18 @@
         <v>9</v>
       </c>
       <c r="D3" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E3" s="2">
-        <v>1</v>
-      </c>
-      <c r="F3" s="2"/>
+        <v>2</v>
+      </c>
+      <c r="F3" s="2">
+        <v>0</v>
+      </c>
       <c r="G3" s="2"/>
       <c r="H3" s="2"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="1" t="s">
         <v>10</v>
       </c>
@@ -1505,16 +1496,18 @@
         <v>12</v>
       </c>
       <c r="D4" s="1">
+        <v>3</v>
+      </c>
+      <c r="E4" s="2">
+        <v>3</v>
+      </c>
+      <c r="F4" s="2">
         <v>1</v>
       </c>
-      <c r="E4" s="2">
-        <v>0</v>
-      </c>
-      <c r="F4" s="2"/>
       <c r="G4" s="2"/>
       <c r="H4" s="2"/>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="1" t="s">
         <v>10</v>
       </c>
@@ -1525,16 +1518,18 @@
         <v>13</v>
       </c>
       <c r="D5" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E5" s="2">
-        <v>0</v>
-      </c>
-      <c r="F5" s="2"/>
+        <v>3</v>
+      </c>
+      <c r="F5" s="2">
+        <v>1</v>
+      </c>
       <c r="G5" s="2"/>
       <c r="H5" s="2"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="1" t="s">
         <v>11</v>
       </c>
@@ -1554,7 +1549,7 @@
       <c r="G6" s="2"/>
       <c r="H6" s="2"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="1" t="s">
         <v>11</v>
       </c>
@@ -1568,13 +1563,13 @@
         <v>2</v>
       </c>
       <c r="E7" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
       <c r="H7" s="2"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="1" t="s">
         <v>16</v>
       </c>
@@ -1594,7 +1589,7 @@
       <c r="G8" s="2"/>
       <c r="H8" s="2"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="1" t="s">
         <v>16</v>
       </c>
@@ -1614,7 +1609,7 @@
       <c r="G9" s="2"/>
       <c r="H9" s="2"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="1" t="s">
         <v>19</v>
       </c>
@@ -1634,7 +1629,7 @@
       <c r="G10" s="2"/>
       <c r="H10" s="2"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="1" t="s">
         <v>19</v>
       </c>
@@ -1654,7 +1649,7 @@
       <c r="G11" s="2"/>
       <c r="H11" s="2"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="1" t="s">
         <v>19</v>
       </c>
@@ -1674,7 +1669,7 @@
       <c r="G12" s="2"/>
       <c r="H12" s="2"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="1" t="s">
         <v>19</v>
       </c>
@@ -1694,7 +1689,7 @@
       <c r="G13" s="2"/>
       <c r="H13" s="2"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" s="1" t="s">
         <v>19</v>
       </c>
@@ -1714,7 +1709,7 @@
       <c r="G14" s="2"/>
       <c r="H14" s="2"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" s="1" t="s">
         <v>19</v>
       </c>
@@ -1734,7 +1729,7 @@
       <c r="G15" s="2"/>
       <c r="H15" s="2"/>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" s="1" t="s">
         <v>35</v>
       </c>
@@ -1754,7 +1749,7 @@
       <c r="G16" s="2"/>
       <c r="H16" s="2"/>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" s="1" t="s">
         <v>19</v>
       </c>
@@ -1774,7 +1769,7 @@
       <c r="G17" s="2"/>
       <c r="H17" s="2"/>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" s="1" t="s">
         <v>19</v>
       </c>
@@ -1794,7 +1789,7 @@
       <c r="G18" s="2"/>
       <c r="H18" s="2"/>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" s="1" t="s">
         <v>19</v>
       </c>
@@ -1814,7 +1809,7 @@
       <c r="G19" s="2"/>
       <c r="H19" s="2"/>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" s="1" t="s">
         <v>19</v>
       </c>
@@ -1834,7 +1829,7 @@
       <c r="G20" s="2"/>
       <c r="H20" s="2"/>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" s="1" t="s">
         <v>30</v>
       </c>
@@ -1854,7 +1849,7 @@
       <c r="G21" s="2"/>
       <c r="H21" s="2"/>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" s="1" t="s">
         <v>30</v>
       </c>
@@ -1874,7 +1869,7 @@
       <c r="G22" s="2"/>
       <c r="H22" s="2"/>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" s="1" t="s">
         <v>30</v>
       </c>
@@ -1894,7 +1889,7 @@
       <c r="G23" s="2"/>
       <c r="H23" s="2"/>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" s="1" t="s">
         <v>30</v>
       </c>
@@ -1914,7 +1909,7 @@
       <c r="G24" s="2"/>
       <c r="H24" s="2"/>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" s="1"/>
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
@@ -1924,7 +1919,7 @@
       <c r="G25" s="2"/>
       <c r="H25" s="2"/>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" s="1"/>
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
@@ -1934,7 +1929,7 @@
       <c r="G26" s="2"/>
       <c r="H26" s="2"/>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" s="1"/>
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
@@ -1944,7 +1939,7 @@
       <c r="G27" s="2"/>
       <c r="H27" s="2"/>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" s="1"/>
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
@@ -1954,21 +1949,21 @@
       <c r="G28" s="2"/>
       <c r="H28" s="2"/>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="C29" s="4" t="s">
         <v>8</v>
       </c>
       <c r="D29" s="3">
         <f>SUM(D3:D28)</f>
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="E29" s="3">
         <f t="shared" ref="E29:H29" si="0">SUM(E3:E28)</f>
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="F29" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G29" s="3">
         <f t="shared" si="0"/>

</xml_diff>

<commit_message>
Sprint Backlog Week2 / Class Diagrams Folder
1) Updated my sprint backlog tasks for week2.
2) Added new folder for class diagrams.
</commit_message>
<xml_diff>
--- a/documentation/Sprint Backlog  Burndown.xlsx
+++ b/documentation/Sprint Backlog  Burndown.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10114"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10211"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/0c751dba731cb2a1/Documents/UWG/2024/Software Engineering 2/Inventory Manager Project/SE2Project/documentation/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/toruggao/Library/CloudStorage/OneDrive-Personal/Documents/UWG/2024/Software Engineering 2/Inventory Manager Project/SE2Project/documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="151" documentId="13_ncr:1_{9C9C4265-351C-41A0-89E5-93A08D9C51A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{28BD0E6D-5362-094C-AE02-20C0C1794EB9}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAA9EC9F-FBCE-5E42-B0DE-C518EF1D6108}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10900" yWindow="1240" windowWidth="29400" windowHeight="17160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="820" windowWidth="29400" windowHeight="17160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="41">
   <si>
     <t>Related User Story</t>
   </si>
@@ -159,9 +159,6 @@
   </si>
   <si>
     <t>JE</t>
-  </si>
-  <si>
-    <t>TBD</t>
   </si>
 </sst>
 </file>
@@ -373,7 +370,7 @@
                   <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0</c:v>
@@ -1156,10 +1153,6 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1428,7 +1421,7 @@
   <dimension ref="A1:H29"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="146" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16:B20"/>
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1670,7 +1663,9 @@
       <c r="E12" s="2">
         <v>0</v>
       </c>
-      <c r="F12" s="2"/>
+      <c r="F12" s="2">
+        <v>1</v>
+      </c>
       <c r="G12" s="2"/>
       <c r="H12" s="2"/>
     </row>
@@ -1690,7 +1685,9 @@
       <c r="E13" s="2">
         <v>0</v>
       </c>
-      <c r="F13" s="2"/>
+      <c r="F13" s="2">
+        <v>1</v>
+      </c>
       <c r="G13" s="2"/>
       <c r="H13" s="2"/>
     </row>
@@ -1710,7 +1707,9 @@
       <c r="E14" s="2">
         <v>0</v>
       </c>
-      <c r="F14" s="2"/>
+      <c r="F14" s="2">
+        <v>0</v>
+      </c>
       <c r="G14" s="2"/>
       <c r="H14" s="2"/>
     </row>
@@ -1730,7 +1729,9 @@
       <c r="E15" s="2">
         <v>0</v>
       </c>
-      <c r="F15" s="2"/>
+      <c r="F15" s="2">
+        <v>1</v>
+      </c>
       <c r="G15" s="2"/>
       <c r="H15" s="2"/>
     </row>
@@ -1739,7 +1740,7 @@
         <v>35</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>36</v>
@@ -1750,7 +1751,9 @@
       <c r="E16" s="2">
         <v>0</v>
       </c>
-      <c r="F16" s="2"/>
+      <c r="F16" s="2">
+        <v>1</v>
+      </c>
       <c r="G16" s="2"/>
       <c r="H16" s="2"/>
     </row>
@@ -1759,7 +1762,7 @@
         <v>19</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>25</v>
@@ -1770,7 +1773,9 @@
       <c r="E17" s="2">
         <v>0</v>
       </c>
-      <c r="F17" s="2"/>
+      <c r="F17" s="2">
+        <v>1</v>
+      </c>
       <c r="G17" s="2"/>
       <c r="H17" s="2"/>
     </row>
@@ -1779,7 +1784,7 @@
         <v>19</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>26</v>
@@ -1790,7 +1795,9 @@
       <c r="E18" s="2">
         <v>0</v>
       </c>
-      <c r="F18" s="2"/>
+      <c r="F18" s="2">
+        <v>0</v>
+      </c>
       <c r="G18" s="2"/>
       <c r="H18" s="2"/>
     </row>
@@ -1799,7 +1806,7 @@
         <v>19</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>27</v>
@@ -1810,7 +1817,9 @@
       <c r="E19" s="2">
         <v>0</v>
       </c>
-      <c r="F19" s="2"/>
+      <c r="F19" s="2">
+        <v>0</v>
+      </c>
       <c r="G19" s="2"/>
       <c r="H19" s="2"/>
     </row>
@@ -1819,7 +1828,7 @@
         <v>19</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>28</v>
@@ -1830,7 +1839,9 @@
       <c r="E20" s="2">
         <v>0</v>
       </c>
-      <c r="F20" s="2"/>
+      <c r="F20" s="2">
+        <v>1</v>
+      </c>
       <c r="G20" s="2"/>
       <c r="H20" s="2"/>
     </row>
@@ -1968,7 +1979,7 @@
       </c>
       <c r="F29" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="G29" s="3">
         <f t="shared" si="0"/>

</xml_diff>

<commit_message>
Update Sprint Backlog Week2
1) Updated time spent on tasks during week 2.
</commit_message>
<xml_diff>
--- a/documentation/Sprint Backlog  Burndown.xlsx
+++ b/documentation/Sprint Backlog  Burndown.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20405"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10211"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jh00291\Documents\GitHub\SE2Project\documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/toruggao/Library/CloudStorage/OneDrive-Personal/Documents/UWG/2024/Software Engineering 2/Inventory Manager Project/SE2Project/documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB62D72E-7584-4929-AAF7-D94ADF2552C0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C54B5FA-2429-DA43-9EBA-0B9542C50462}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10905" yWindow="1245" windowWidth="29400" windowHeight="17160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="820" windowWidth="29400" windowHeight="17160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,12 +20,23 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="41">
   <si>
     <t>Related User Story</t>
   </si>
@@ -148,9 +159,6 @@
   </si>
   <si>
     <t>JE</t>
-  </si>
-  <si>
-    <t>TBD</t>
   </si>
 </sst>
 </file>
@@ -359,10 +367,10 @@
                   <c:v>46</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>11</c:v>
+                  <c:v>27</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0</c:v>
@@ -1145,10 +1153,6 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1417,17 +1421,17 @@
   <dimension ref="A1:H29"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="146" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="2" width="26" customWidth="1"/>
-    <col min="3" max="3" width="41.7109375" customWidth="1"/>
-    <col min="4" max="4" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="41.6640625" customWidth="1"/>
+    <col min="4" max="4" width="14.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
@@ -1445,7 +1449,7 @@
       <c r="G1" s="7"/>
       <c r="H1" s="7"/>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="8"/>
       <c r="B2" s="6"/>
       <c r="C2" s="8"/>
@@ -1463,7 +1467,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>10</v>
       </c>
@@ -1483,7 +1487,7 @@
       <c r="G3" s="2"/>
       <c r="H3" s="2"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>10</v>
       </c>
@@ -1503,7 +1507,7 @@
       <c r="G4" s="2"/>
       <c r="H4" s="2"/>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>10</v>
       </c>
@@ -1523,7 +1527,7 @@
       <c r="G5" s="2"/>
       <c r="H5" s="2"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>11</v>
       </c>
@@ -1545,7 +1549,7 @@
       <c r="G6" s="2"/>
       <c r="H6" s="2"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>11</v>
       </c>
@@ -1567,7 +1571,7 @@
       <c r="G7" s="2"/>
       <c r="H7" s="2"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>16</v>
       </c>
@@ -1587,7 +1591,7 @@
       <c r="G8" s="2"/>
       <c r="H8" s="2"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>16</v>
       </c>
@@ -1607,7 +1611,7 @@
       <c r="G9" s="2"/>
       <c r="H9" s="2"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>19</v>
       </c>
@@ -1621,13 +1625,15 @@
         <v>1</v>
       </c>
       <c r="E10" s="2">
-        <v>1</v>
-      </c>
-      <c r="F10" s="2"/>
+        <v>0</v>
+      </c>
+      <c r="F10" s="2">
+        <v>0</v>
+      </c>
       <c r="G10" s="2"/>
       <c r="H10" s="2"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>19</v>
       </c>
@@ -1641,13 +1647,15 @@
         <v>1</v>
       </c>
       <c r="E11" s="2">
-        <v>0</v>
-      </c>
-      <c r="F11" s="2"/>
+        <v>1</v>
+      </c>
+      <c r="F11" s="2">
+        <v>1</v>
+      </c>
       <c r="G11" s="2"/>
       <c r="H11" s="2"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>19</v>
       </c>
@@ -1661,13 +1669,15 @@
         <v>2</v>
       </c>
       <c r="E12" s="2">
-        <v>0</v>
-      </c>
-      <c r="F12" s="2"/>
+        <v>1</v>
+      </c>
+      <c r="F12" s="2">
+        <v>1</v>
+      </c>
       <c r="G12" s="2"/>
       <c r="H12" s="2"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>19</v>
       </c>
@@ -1681,13 +1691,15 @@
         <v>2</v>
       </c>
       <c r="E13" s="2">
-        <v>0</v>
-      </c>
-      <c r="F13" s="2"/>
+        <v>1</v>
+      </c>
+      <c r="F13" s="2">
+        <v>1</v>
+      </c>
       <c r="G13" s="2"/>
       <c r="H13" s="2"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>19</v>
       </c>
@@ -1701,13 +1713,15 @@
         <v>2</v>
       </c>
       <c r="E14" s="2">
-        <v>0</v>
-      </c>
-      <c r="F14" s="2"/>
+        <v>2</v>
+      </c>
+      <c r="F14" s="2">
+        <v>1</v>
+      </c>
       <c r="G14" s="2"/>
       <c r="H14" s="2"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>19</v>
       </c>
@@ -1721,18 +1735,20 @@
         <v>2</v>
       </c>
       <c r="E15" s="2">
-        <v>0</v>
-      </c>
-      <c r="F15" s="2"/>
+        <v>1</v>
+      </c>
+      <c r="F15" s="2">
+        <v>1</v>
+      </c>
       <c r="G15" s="2"/>
       <c r="H15" s="2"/>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>35</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>36</v>
@@ -1741,18 +1757,20 @@
         <v>3</v>
       </c>
       <c r="E16" s="2">
-        <v>0</v>
-      </c>
-      <c r="F16" s="2"/>
+        <v>3</v>
+      </c>
+      <c r="F16" s="2">
+        <v>1</v>
+      </c>
       <c r="G16" s="2"/>
       <c r="H16" s="2"/>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>19</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>25</v>
@@ -1761,18 +1779,20 @@
         <v>2</v>
       </c>
       <c r="E17" s="2">
-        <v>0</v>
-      </c>
-      <c r="F17" s="2"/>
+        <v>2</v>
+      </c>
+      <c r="F17" s="2">
+        <v>1</v>
+      </c>
       <c r="G17" s="2"/>
       <c r="H17" s="2"/>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>19</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>26</v>
@@ -1781,18 +1801,20 @@
         <v>2</v>
       </c>
       <c r="E18" s="2">
-        <v>0</v>
-      </c>
-      <c r="F18" s="2"/>
+        <v>2</v>
+      </c>
+      <c r="F18" s="2">
+        <v>1</v>
+      </c>
       <c r="G18" s="2"/>
       <c r="H18" s="2"/>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>19</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>27</v>
@@ -1801,18 +1823,20 @@
         <v>2</v>
       </c>
       <c r="E19" s="2">
-        <v>0</v>
-      </c>
-      <c r="F19" s="2"/>
+        <v>2</v>
+      </c>
+      <c r="F19" s="2">
+        <v>1</v>
+      </c>
       <c r="G19" s="2"/>
       <c r="H19" s="2"/>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>19</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>28</v>
@@ -1821,13 +1845,15 @@
         <v>2</v>
       </c>
       <c r="E20" s="2">
-        <v>0</v>
-      </c>
-      <c r="F20" s="2"/>
+        <v>2</v>
+      </c>
+      <c r="F20" s="2">
+        <v>1</v>
+      </c>
       <c r="G20" s="2"/>
       <c r="H20" s="2"/>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>30</v>
       </c>
@@ -1847,7 +1873,7 @@
       <c r="G21" s="2"/>
       <c r="H21" s="2"/>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>30</v>
       </c>
@@ -1867,7 +1893,7 @@
       <c r="G22" s="2"/>
       <c r="H22" s="2"/>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>30</v>
       </c>
@@ -1887,7 +1913,7 @@
       <c r="G23" s="2"/>
       <c r="H23" s="2"/>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>30</v>
       </c>
@@ -1907,7 +1933,7 @@
       <c r="G24" s="2"/>
       <c r="H24" s="2"/>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A25" s="1"/>
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
@@ -1917,7 +1943,7 @@
       <c r="G25" s="2"/>
       <c r="H25" s="2"/>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A26" s="1"/>
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
@@ -1927,7 +1953,7 @@
       <c r="G26" s="2"/>
       <c r="H26" s="2"/>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A27" s="1"/>
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
@@ -1937,7 +1963,7 @@
       <c r="G27" s="2"/>
       <c r="H27" s="2"/>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A28" s="1"/>
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
@@ -1947,7 +1973,7 @@
       <c r="G28" s="2"/>
       <c r="H28" s="2"/>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C29" s="4" t="s">
         <v>8</v>
       </c>
@@ -1957,11 +1983,11 @@
       </c>
       <c r="E29" s="3">
         <f t="shared" ref="E29:H29" si="0">SUM(E3:E28)</f>
-        <v>11</v>
+        <v>27</v>
       </c>
       <c r="F29" s="3">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="G29" s="3">
         <f t="shared" si="0"/>

</xml_diff>

<commit_message>
Update Sprint backlog Hours
1) Update hours spent on tasks
</commit_message>
<xml_diff>
--- a/documentation/Sprint Backlog  Burndown.xlsx
+++ b/documentation/Sprint Backlog  Burndown.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20405"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10211"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jn00041\Documents\GitHub\SE2Project\documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/toruggao/Library/CloudStorage/OneDrive-Personal/Documents/UWG/2024/Software Engineering 2/Inventory Manager Project/SE2Project/documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9EB2103-DF34-4450-91F8-386221988455}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BB774ED-A98C-AB40-8B28-581984FE53D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="0" windowWidth="11460" windowHeight="14415" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="22700" windowHeight="14420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,6 +19,17 @@
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -359,13 +370,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>53</c:v>
+                  <c:v>60</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>47</c:v>
+                  <c:v>49</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>25</c:v>
+                  <c:v>26</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0</c:v>
@@ -1415,18 +1426,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H31"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView tabSelected="1" zoomScale="69" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="2" width="26" customWidth="1"/>
-    <col min="3" max="3" width="41.5703125" customWidth="1"/>
-    <col min="4" max="4" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="41.5" customWidth="1"/>
+    <col min="4" max="4" width="14.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
@@ -1444,7 +1455,7 @@
       <c r="G1" s="7"/>
       <c r="H1" s="7"/>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="8"/>
       <c r="B2" s="6"/>
       <c r="C2" s="8"/>
@@ -1462,7 +1473,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>10</v>
       </c>
@@ -1484,7 +1495,7 @@
       <c r="G3" s="2"/>
       <c r="H3" s="2"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>10</v>
       </c>
@@ -1506,7 +1517,7 @@
       <c r="G4" s="2"/>
       <c r="H4" s="2"/>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>10</v>
       </c>
@@ -1528,7 +1539,7 @@
       <c r="G5" s="2"/>
       <c r="H5" s="2"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>11</v>
       </c>
@@ -1550,7 +1561,7 @@
       <c r="G6" s="2"/>
       <c r="H6" s="2"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>11</v>
       </c>
@@ -1572,7 +1583,7 @@
       <c r="G7" s="2"/>
       <c r="H7" s="2"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>16</v>
       </c>
@@ -1594,7 +1605,7 @@
       <c r="G8" s="2"/>
       <c r="H8" s="2"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>16</v>
       </c>
@@ -1616,7 +1627,7 @@
       <c r="G9" s="2"/>
       <c r="H9" s="2"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>19</v>
       </c>
@@ -1638,7 +1649,7 @@
       <c r="G10" s="2"/>
       <c r="H10" s="2"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>19</v>
       </c>
@@ -1660,7 +1671,7 @@
       <c r="G11" s="2"/>
       <c r="H11" s="2"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>19</v>
       </c>
@@ -1671,10 +1682,10 @@
         <v>21</v>
       </c>
       <c r="D12" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E12" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F12" s="2">
         <v>1</v>
@@ -1682,7 +1693,7 @@
       <c r="G12" s="2"/>
       <c r="H12" s="2"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>19</v>
       </c>
@@ -1693,10 +1704,10 @@
         <v>22</v>
       </c>
       <c r="D13" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E13" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F13" s="2">
         <v>1</v>
@@ -1704,7 +1715,7 @@
       <c r="G13" s="2"/>
       <c r="H13" s="2"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>19</v>
       </c>
@@ -1721,12 +1732,12 @@
         <v>2</v>
       </c>
       <c r="F14" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G14" s="2"/>
       <c r="H14" s="2"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>19</v>
       </c>
@@ -1737,10 +1748,10 @@
         <v>24</v>
       </c>
       <c r="D15" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E15" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F15" s="2">
         <v>1</v>
@@ -1748,7 +1759,7 @@
       <c r="G15" s="2"/>
       <c r="H15" s="2"/>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>35</v>
       </c>
@@ -1762,7 +1773,7 @@
         <v>3</v>
       </c>
       <c r="E16" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F16" s="2">
         <v>1</v>
@@ -1770,7 +1781,7 @@
       <c r="G16" s="2"/>
       <c r="H16" s="2"/>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>19</v>
       </c>
@@ -1781,7 +1792,7 @@
         <v>25</v>
       </c>
       <c r="D17" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E17" s="2">
         <v>2</v>
@@ -1792,7 +1803,7 @@
       <c r="G17" s="2"/>
       <c r="H17" s="2"/>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>19</v>
       </c>
@@ -1803,7 +1814,7 @@
         <v>26</v>
       </c>
       <c r="D18" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E18" s="2">
         <v>2</v>
@@ -1814,7 +1825,7 @@
       <c r="G18" s="2"/>
       <c r="H18" s="2"/>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>19</v>
       </c>
@@ -1825,7 +1836,7 @@
         <v>27</v>
       </c>
       <c r="D19" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E19" s="2">
         <v>2</v>
@@ -1836,7 +1847,7 @@
       <c r="G19" s="2"/>
       <c r="H19" s="2"/>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>19</v>
       </c>
@@ -1847,7 +1858,7 @@
         <v>28</v>
       </c>
       <c r="D20" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E20" s="2">
         <v>2</v>
@@ -1858,7 +1869,7 @@
       <c r="G20" s="2"/>
       <c r="H20" s="2"/>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>30</v>
       </c>
@@ -1880,7 +1891,7 @@
       <c r="G21" s="2"/>
       <c r="H21" s="2"/>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>30</v>
       </c>
@@ -1902,7 +1913,7 @@
       <c r="G22" s="2"/>
       <c r="H22" s="2"/>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>30</v>
       </c>
@@ -1924,7 +1935,7 @@
       <c r="G23" s="2"/>
       <c r="H23" s="2"/>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>30</v>
       </c>
@@ -1946,7 +1957,7 @@
       <c r="G24" s="2"/>
       <c r="H24" s="2"/>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
         <v>30</v>
       </c>
@@ -1968,7 +1979,7 @@
       <c r="G25" s="2"/>
       <c r="H25" s="2"/>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
         <v>30</v>
       </c>
@@ -1990,7 +2001,7 @@
       <c r="G26" s="2"/>
       <c r="H26" s="2"/>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A27" s="1"/>
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
@@ -2000,7 +2011,7 @@
       <c r="G27" s="2"/>
       <c r="H27" s="2"/>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A28" s="1"/>
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
@@ -2010,7 +2021,7 @@
       <c r="G28" s="2"/>
       <c r="H28" s="2"/>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A29" s="1"/>
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
@@ -2020,7 +2031,7 @@
       <c r="G29" s="2"/>
       <c r="H29" s="2"/>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A30" s="1"/>
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
@@ -2030,21 +2041,21 @@
       <c r="G30" s="2"/>
       <c r="H30" s="2"/>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C31" s="4" t="s">
         <v>8</v>
       </c>
       <c r="D31" s="3">
         <f>SUM(D3:D30)</f>
-        <v>53</v>
+        <v>60</v>
       </c>
       <c r="E31" s="3">
         <f t="shared" ref="E31:H31" si="0">SUM(E3:E30)</f>
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="F31" s="3">
         <f t="shared" si="0"/>
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="G31" s="3">
         <f t="shared" si="0"/>

</xml_diff>

<commit_message>
Restructured Test Packages / Fix Classpath
1) Restructured test packages for better presentation.
2) Fix class path so matches the team configuration.
</commit_message>
<xml_diff>
--- a/documentation/Sprint Backlog  Burndown.xlsx
+++ b/documentation/Sprint Backlog  Burndown.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10114"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10211"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/0c751dba731cb2a1/Documents/UWG/2024/Software Engineering 2/Inventory Manager Project/SE2Project/documentation/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/toruggao/Library/CloudStorage/OneDrive-Personal/Documents/UWG/2024/Software Engineering 2/Inventory Manager Project/SE2Project/documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="151" documentId="13_ncr:1_{9C9C4265-351C-41A0-89E5-93A08D9C51A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{28BD0E6D-5362-094C-AE02-20C0C1794EB9}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB9D5B51-3304-6845-8CAD-3191E20B05C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10900" yWindow="1240" windowWidth="29400" windowHeight="17160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20" yWindow="740" windowWidth="29400" windowHeight="17240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="44">
   <si>
     <t>Related User Story</t>
   </si>
@@ -161,7 +161,13 @@
     <t>JE</t>
   </si>
   <si>
-    <t>TBD</t>
+    <t>Implement functionality for orders</t>
+  </si>
+  <si>
+    <t>Testing for orders functionality</t>
+  </si>
+  <si>
+    <t>Create Model Class for inventory</t>
   </si>
 </sst>
 </file>
@@ -362,18 +368,18 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$D$29:$H$29</c:f>
+              <c:f>Sheet1!$D$32:$H$32</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>42</c:v>
+                  <c:v>63</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5</c:v>
+                  <c:v>50</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>28</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0</c:v>
@@ -1156,10 +1162,6 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1425,16 +1427,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H29"/>
+  <dimension ref="A1:H32"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="146" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16:B20"/>
+    <sheetView tabSelected="1" zoomScale="135" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="2" width="26" customWidth="1"/>
-    <col min="3" max="3" width="41.6640625" customWidth="1"/>
+    <col min="3" max="3" width="41.5" customWidth="1"/>
     <col min="4" max="4" width="14.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1490,7 +1492,9 @@
       <c r="E3" s="2">
         <v>1</v>
       </c>
-      <c r="F3" s="2"/>
+      <c r="F3" s="2">
+        <v>0</v>
+      </c>
       <c r="G3" s="2"/>
       <c r="H3" s="2"/>
     </row>
@@ -1505,12 +1509,14 @@
         <v>12</v>
       </c>
       <c r="D4" s="1">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E4" s="2">
-        <v>0</v>
-      </c>
-      <c r="F4" s="2"/>
+        <v>4</v>
+      </c>
+      <c r="F4" s="2">
+        <v>1</v>
+      </c>
       <c r="G4" s="2"/>
       <c r="H4" s="2"/>
     </row>
@@ -1525,12 +1531,14 @@
         <v>13</v>
       </c>
       <c r="D5" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E5" s="2">
-        <v>0</v>
-      </c>
-      <c r="F5" s="2"/>
+        <v>2</v>
+      </c>
+      <c r="F5" s="2">
+        <v>1</v>
+      </c>
       <c r="G5" s="2"/>
       <c r="H5" s="2"/>
     </row>
@@ -1550,7 +1558,9 @@
       <c r="E6" s="2">
         <v>1</v>
       </c>
-      <c r="F6" s="2"/>
+      <c r="F6" s="2">
+        <v>0</v>
+      </c>
       <c r="G6" s="2"/>
       <c r="H6" s="2"/>
     </row>
@@ -1565,12 +1575,14 @@
         <v>15</v>
       </c>
       <c r="D7" s="1">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="E7" s="2">
-        <v>0</v>
-      </c>
-      <c r="F7" s="2"/>
+        <v>6</v>
+      </c>
+      <c r="F7" s="2">
+        <v>3</v>
+      </c>
       <c r="G7" s="2"/>
       <c r="H7" s="2"/>
     </row>
@@ -1590,7 +1602,9 @@
       <c r="E8" s="2">
         <v>1</v>
       </c>
-      <c r="F8" s="2"/>
+      <c r="F8" s="2">
+        <v>0</v>
+      </c>
       <c r="G8" s="2"/>
       <c r="H8" s="2"/>
     </row>
@@ -1608,9 +1622,11 @@
         <v>3</v>
       </c>
       <c r="E9" s="2">
-        <v>0</v>
-      </c>
-      <c r="F9" s="2"/>
+        <v>3</v>
+      </c>
+      <c r="F9" s="2">
+        <v>3</v>
+      </c>
       <c r="G9" s="2"/>
       <c r="H9" s="2"/>
     </row>
@@ -1628,9 +1644,11 @@
         <v>1</v>
       </c>
       <c r="E10" s="2">
-        <v>1</v>
-      </c>
-      <c r="F10" s="2"/>
+        <v>0</v>
+      </c>
+      <c r="F10" s="2">
+        <v>0</v>
+      </c>
       <c r="G10" s="2"/>
       <c r="H10" s="2"/>
     </row>
@@ -1648,9 +1666,11 @@
         <v>1</v>
       </c>
       <c r="E11" s="2">
-        <v>0</v>
-      </c>
-      <c r="F11" s="2"/>
+        <v>1</v>
+      </c>
+      <c r="F11" s="2">
+        <v>1</v>
+      </c>
       <c r="G11" s="2"/>
       <c r="H11" s="2"/>
     </row>
@@ -1665,12 +1685,14 @@
         <v>21</v>
       </c>
       <c r="D12" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E12" s="2">
-        <v>0</v>
-      </c>
-      <c r="F12" s="2"/>
+        <v>2</v>
+      </c>
+      <c r="F12" s="2">
+        <v>1</v>
+      </c>
       <c r="G12" s="2"/>
       <c r="H12" s="2"/>
     </row>
@@ -1685,12 +1707,14 @@
         <v>22</v>
       </c>
       <c r="D13" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E13" s="2">
-        <v>0</v>
-      </c>
-      <c r="F13" s="2"/>
+        <v>2</v>
+      </c>
+      <c r="F13" s="2">
+        <v>1</v>
+      </c>
       <c r="G13" s="2"/>
       <c r="H13" s="2"/>
     </row>
@@ -1708,9 +1732,11 @@
         <v>2</v>
       </c>
       <c r="E14" s="2">
-        <v>0</v>
-      </c>
-      <c r="F14" s="2"/>
+        <v>2</v>
+      </c>
+      <c r="F14" s="2">
+        <v>2</v>
+      </c>
       <c r="G14" s="2"/>
       <c r="H14" s="2"/>
     </row>
@@ -1725,12 +1751,14 @@
         <v>24</v>
       </c>
       <c r="D15" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E15" s="2">
-        <v>0</v>
-      </c>
-      <c r="F15" s="2"/>
+        <v>2</v>
+      </c>
+      <c r="F15" s="2">
+        <v>1</v>
+      </c>
       <c r="G15" s="2"/>
       <c r="H15" s="2"/>
     </row>
@@ -1739,7 +1767,7 @@
         <v>35</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>36</v>
@@ -1748,9 +1776,11 @@
         <v>3</v>
       </c>
       <c r="E16" s="2">
-        <v>0</v>
-      </c>
-      <c r="F16" s="2"/>
+        <v>2</v>
+      </c>
+      <c r="F16" s="2">
+        <v>1</v>
+      </c>
       <c r="G16" s="2"/>
       <c r="H16" s="2"/>
     </row>
@@ -1759,18 +1789,20 @@
         <v>19</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>25</v>
       </c>
       <c r="D17" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E17" s="2">
-        <v>0</v>
-      </c>
-      <c r="F17" s="2"/>
+        <v>2</v>
+      </c>
+      <c r="F17" s="2">
+        <v>1</v>
+      </c>
       <c r="G17" s="2"/>
       <c r="H17" s="2"/>
     </row>
@@ -1779,18 +1811,20 @@
         <v>19</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>26</v>
       </c>
       <c r="D18" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E18" s="2">
-        <v>0</v>
-      </c>
-      <c r="F18" s="2"/>
+        <v>2</v>
+      </c>
+      <c r="F18" s="2">
+        <v>1</v>
+      </c>
       <c r="G18" s="2"/>
       <c r="H18" s="2"/>
     </row>
@@ -1799,18 +1833,20 @@
         <v>19</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>27</v>
       </c>
       <c r="D19" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E19" s="2">
-        <v>0</v>
-      </c>
-      <c r="F19" s="2"/>
+        <v>2</v>
+      </c>
+      <c r="F19" s="2">
+        <v>1</v>
+      </c>
       <c r="G19" s="2"/>
       <c r="H19" s="2"/>
     </row>
@@ -1819,38 +1855,42 @@
         <v>19</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>28</v>
       </c>
       <c r="D20" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E20" s="2">
-        <v>0</v>
-      </c>
-      <c r="F20" s="2"/>
+        <v>2</v>
+      </c>
+      <c r="F20" s="2">
+        <v>1</v>
+      </c>
       <c r="G20" s="2"/>
       <c r="H20" s="2"/>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
-        <v>30</v>
+        <v>19</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>31</v>
+        <v>43</v>
       </c>
       <c r="D21" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E21" s="2">
         <v>1</v>
       </c>
-      <c r="F21" s="2"/>
+      <c r="F21" s="2">
+        <v>2</v>
+      </c>
       <c r="G21" s="2"/>
       <c r="H21" s="2"/>
     </row>
@@ -1862,15 +1902,17 @@
         <v>40</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D22" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E22" s="2">
+        <v>1</v>
+      </c>
+      <c r="F22" s="2">
         <v>0</v>
       </c>
-      <c r="F22" s="2"/>
       <c r="G22" s="2"/>
       <c r="H22" s="2"/>
     </row>
@@ -1882,15 +1924,17 @@
         <v>40</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>33</v>
+        <v>41</v>
       </c>
       <c r="D23" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E23" s="2">
+        <v>2</v>
+      </c>
+      <c r="F23" s="2">
         <v>0</v>
       </c>
-      <c r="F23" s="2"/>
       <c r="G23" s="2"/>
       <c r="H23" s="2"/>
     </row>
@@ -1902,45 +1946,81 @@
         <v>40</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>34</v>
+        <v>42</v>
       </c>
       <c r="D24" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E24" s="2">
+        <v>2</v>
+      </c>
+      <c r="F24" s="2">
         <v>0</v>
       </c>
-      <c r="F24" s="2"/>
       <c r="G24" s="2"/>
       <c r="H24" s="2"/>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A25" s="1"/>
-      <c r="B25" s="1"/>
-      <c r="C25" s="1"/>
-      <c r="D25" s="1"/>
-      <c r="E25" s="2"/>
-      <c r="F25" s="2"/>
+      <c r="A25" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D25" s="1">
+        <v>2</v>
+      </c>
+      <c r="E25" s="2">
+        <v>2</v>
+      </c>
+      <c r="F25" s="2">
+        <v>2</v>
+      </c>
       <c r="G25" s="2"/>
       <c r="H25" s="2"/>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A26" s="1"/>
-      <c r="B26" s="1"/>
-      <c r="C26" s="1"/>
-      <c r="D26" s="1"/>
-      <c r="E26" s="2"/>
-      <c r="F26" s="2"/>
+      <c r="A26" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D26" s="1">
+        <v>2</v>
+      </c>
+      <c r="E26" s="2">
+        <v>2</v>
+      </c>
+      <c r="F26" s="2">
+        <v>2</v>
+      </c>
       <c r="G26" s="2"/>
       <c r="H26" s="2"/>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A27" s="1"/>
+      <c r="A27" s="1" t="s">
+        <v>30</v>
+      </c>
       <c r="B27" s="1"/>
-      <c r="C27" s="1"/>
-      <c r="D27" s="1"/>
-      <c r="E27" s="2"/>
-      <c r="F27" s="2"/>
+      <c r="C27" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D27" s="1">
+        <v>3</v>
+      </c>
+      <c r="E27" s="2">
+        <v>3</v>
+      </c>
+      <c r="F27" s="2">
+        <v>3</v>
+      </c>
       <c r="G27" s="2"/>
       <c r="H27" s="2"/>
     </row>
@@ -1955,26 +2035,56 @@
       <c r="H28" s="2"/>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="C29" s="4" t="s">
+      <c r="A29" s="1"/>
+      <c r="B29" s="1"/>
+      <c r="C29" s="1"/>
+      <c r="D29" s="1"/>
+      <c r="E29" s="2"/>
+      <c r="F29" s="2"/>
+      <c r="G29" s="2"/>
+      <c r="H29" s="2"/>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A30" s="1"/>
+      <c r="B30" s="1"/>
+      <c r="C30" s="1"/>
+      <c r="D30" s="1"/>
+      <c r="E30" s="2"/>
+      <c r="F30" s="2"/>
+      <c r="G30" s="2"/>
+      <c r="H30" s="2"/>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A31" s="1"/>
+      <c r="B31" s="1"/>
+      <c r="C31" s="1"/>
+      <c r="D31" s="1"/>
+      <c r="E31" s="2"/>
+      <c r="F31" s="2"/>
+      <c r="G31" s="2"/>
+      <c r="H31" s="2"/>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="C32" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="D29" s="3">
-        <f>SUM(D3:D28)</f>
-        <v>42</v>
-      </c>
-      <c r="E29" s="3">
-        <f t="shared" ref="E29:H29" si="0">SUM(E3:E28)</f>
-        <v>5</v>
-      </c>
-      <c r="F29" s="3">
+      <c r="D32" s="3">
+        <f>SUM(D3:D31)</f>
+        <v>63</v>
+      </c>
+      <c r="E32" s="3">
+        <f t="shared" ref="E32:H32" si="0">SUM(E3:E31)</f>
+        <v>50</v>
+      </c>
+      <c r="F32" s="3">
+        <f t="shared" si="0"/>
+        <v>28</v>
+      </c>
+      <c r="G32" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G29" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="H29" s="3">
+      <c r="H32" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>

</xml_diff>